<commit_message>
added switch configuration by signal
</commit_message>
<xml_diff>
--- a/device/連動図表_柴山.xlsx
+++ b/device/連動図表_柴山.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D6C233-8BDF-47BC-A6DF-B7C7051E77D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0182F44-717F-4E7D-A3B4-E7920A4B308E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="メモ" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -269,33 +270,39 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>○21</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>21, (〇31片)</t>
+    <t>31T,2RT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>〇31</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>21, (〇31片, 〇4L片)</t>
     <rPh sb="8" eb="9">
       <t>カタ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>31, (〇21片)</t>
+    <rPh sb="14" eb="15">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>31, (〇21片, 〇3R片)</t>
     <rPh sb="8" eb="9">
       <t>カタ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>31T,2RT</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>〇31</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>5R</t>
+    <rPh sb="14" eb="15">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>〇21</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1876,6 +1883,99 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>284903</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>170208</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4AC7396-1C22-4174-A681-24709DD61FA4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5857875" y="0"/>
+          <a:ext cx="6771428" cy="9933333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>618278</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>170208</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="図 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E27E6C14-AD2F-4ED4-AD38-DF861D4AB67A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19050" y="0"/>
+          <a:ext cx="6771428" cy="9933333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2146,8 +2246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:AN22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="15.75"/>
@@ -2166,7 +2266,7 @@
     </row>
     <row r="4" spans="3:40">
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="3:40">
@@ -2246,7 +2346,7 @@
         <v>2</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="AA17" s="1" t="s">
         <v>23</v>
@@ -2271,7 +2371,7 @@
         <v>1</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="AA19" s="1" t="s">
         <v>24</v>
@@ -2291,10 +2391,10 @@
         <v>0</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="AA20" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="AI20" s="1" t="s">
         <v>25</v>
@@ -2316,7 +2416,7 @@
         <v>3</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AA22" s="1" t="s">
         <v>25</v>
@@ -2331,4 +2431,21 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F23A584-8EFB-4D7F-A3A1-CAC64E545BCA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M43" sqref="M42:M43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed control to route signal
</commit_message>
<xml_diff>
--- a/device/連動図表_柴山.xlsx
+++ b/device/連動図表_柴山.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0182F44-717F-4E7D-A3B4-E7920A4B308E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED4223C-DA0D-4DD6-871D-ADB39AA6ED0F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,21 +21,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
-  <si>
-    <t>5R</t>
-    <phoneticPr fontId="1"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>3R</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>2L</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>4L</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -270,39 +262,108 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>31T,2RT</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>〇31</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>5R</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>21, (〇31片, 〇4L片)</t>
+    <t>〇21</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>保留鎖錠</t>
+    <rPh sb="0" eb="2">
+      <t>ホリュウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>サジョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>30秒</t>
+    <rPh sb="2" eb="3">
+      <t>ビョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>31T, 2RT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3L</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>開通てこ</t>
+    <rPh sb="0" eb="2">
+      <t>カイツウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2番線～京都方</t>
+    <rPh sb="1" eb="2">
+      <t>バン</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>セン</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>キョウト</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1番線～幡生方</t>
+    <rPh sb="1" eb="2">
+      <t>バン</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>セン</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ハタブ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>11L</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>11R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(〇31片, 〇4L片)</t>
+  </si>
+  <si>
+    <t>(〇21片, 〇3R片)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">31, 〇11R片 </t>
     <rPh sb="8" eb="9">
       <t>カタ</t>
     </rPh>
-    <rPh sb="14" eb="15">
-      <t>カタ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>31, (〇21片, 〇3R片)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>21, 〇11L片</t>
     <rPh sb="8" eb="9">
       <t>カタ</t>
     </rPh>
-    <rPh sb="14" eb="15">
-      <t>カタ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>〇21</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -430,495 +491,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>39385</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>78769</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="グループ化 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C068783-9167-4911-982E-530A3FF5CA13}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="993913" y="834515"/>
-          <a:ext cx="596348" cy="238167"/>
-          <a:chOff x="993913" y="834515"/>
-          <a:chExt cx="596348" cy="238167"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="7" name="直線コネクタ 6">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C40ACFB-1A80-44B3-A4D0-CCFB251E7E43}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="993913" y="834515"/>
-            <a:ext cx="0" cy="238167"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="10" name="楕円 9">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2F6F893-3940-4525-8DF3-2322028CB3FF}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1351722" y="834515"/>
-            <a:ext cx="238539" cy="238167"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="12" name="直線コネクタ 11">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A0C7496-D05A-458F-9E20-518A49C21ED2}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:endCxn id="10" idx="2"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="993913" y="953598"/>
-            <a:ext cx="357809" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>40005</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="36" name="グループ化 35">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F3BE561-A324-4FF7-9672-48610E497971}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="5565913" y="795130"/>
-          <a:ext cx="596348" cy="238788"/>
-          <a:chOff x="5610225" y="760095"/>
-          <a:chExt cx="600075" cy="240030"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="30" name="直線コネクタ 29">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0E6B766-0DE6-45BD-AC07-0412665313F1}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5610225" y="760095"/>
-            <a:ext cx="0" cy="240030"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="32" name="楕円 31">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55C74513-4114-48D8-8BCB-C1C6A1952826}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5970270" y="760095"/>
-            <a:ext cx="240030" cy="240030"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="33" name="直線コネクタ 32">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BE5B69-70F6-4C7A-83DC-234DC92DCF0F}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:endCxn id="32" idx="2"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5610225" y="880110"/>
-            <a:ext cx="360045" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>11430</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="37" name="グループ化 36">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B363EB48-221F-4245-90BA-C1B7861D499C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm flipH="1">
-          <a:off x="2186609" y="1960493"/>
-          <a:ext cx="596348" cy="237546"/>
-          <a:chOff x="5600700" y="1354455"/>
-          <a:chExt cx="600075" cy="240030"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="38" name="直線コネクタ 37">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFE19FE8-7A8F-4D09-A4A4-68AB7BD1E714}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5600700" y="1354455"/>
-            <a:ext cx="0" cy="240030"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="39" name="楕円 38">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E1DE7B8-7105-4567-A8CA-BE599B7E04B6}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5960745" y="1354455"/>
-            <a:ext cx="240030" cy="240030"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="40" name="直線コネクタ 39">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D99BD293-477B-47C5-847F-7B71E02BED49}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:endCxn id="39" idx="2"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5600700" y="1474470"/>
-            <a:ext cx="360045" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>5</xdr:row>
@@ -943,8 +515,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1733136" y="1097446"/>
-          <a:ext cx="208307" cy="95250"/>
+          <a:off x="1719427" y="1088878"/>
+          <a:ext cx="206594" cy="93536"/>
           <a:chOff x="6400800" y="2200275"/>
           <a:chExt cx="600075" cy="200025"/>
         </a:xfrm>
@@ -1098,8 +670,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6437243" y="1789043"/>
-          <a:ext cx="208308" cy="95250"/>
+          <a:off x="6382407" y="1775334"/>
+          <a:ext cx="206594" cy="93537"/>
           <a:chOff x="6400800" y="2200275"/>
           <a:chExt cx="600075" cy="200025"/>
         </a:xfrm>
@@ -1559,169 +1131,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>126267</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>165651</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="18" name="グループ化 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCC2D9E8-D506-4866-B248-5C25CE9763FF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="6957391" y="2114093"/>
-          <a:ext cx="596348" cy="238167"/>
-          <a:chOff x="6957391" y="1352095"/>
-          <a:chExt cx="596348" cy="238167"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="71" name="直線コネクタ 70">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{286386E9-B774-4FEB-A881-4F6431EC922B}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1">
-            <a:off x="7553739" y="1352095"/>
-            <a:ext cx="0" cy="238167"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="73" name="楕円 72">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C23E349A-B53B-4933-B7B4-64E4FB4A2265}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1">
-            <a:off x="6957391" y="1352095"/>
-            <a:ext cx="238539" cy="238167"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="74" name="直線コネクタ 73">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{883FCCA8-2A64-4DEB-A44D-14AD6A7DC7C5}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:endCxn id="73" idx="2"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1">
-            <a:off x="7195930" y="1471178"/>
-            <a:ext cx="357809" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>41414</xdr:colOff>
       <xdr:row>5</xdr:row>
@@ -1883,6 +1292,1298 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>195513</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>191438</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>194146</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>30295</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="31" name="グループ化 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{002C8C29-FCE6-4D8F-A215-E8A3197E111A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm flipH="1">
+          <a:off x="983789" y="782645"/>
+          <a:ext cx="589840" cy="232995"/>
+          <a:chOff x="6970568" y="2117858"/>
+          <a:chExt cx="597477" cy="238543"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="18" name="グループ化 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCC2D9E8-D506-4866-B248-5C25CE9763FF}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="6970568" y="2117858"/>
+            <a:ext cx="597477" cy="238543"/>
+            <a:chOff x="6957391" y="1352095"/>
+            <a:chExt cx="596348" cy="238167"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="71" name="直線コネクタ 70">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{286386E9-B774-4FEB-A881-4F6431EC922B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="7553739" y="1352095"/>
+              <a:ext cx="0" cy="238167"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="73" name="楕円 72">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C23E349A-B53B-4933-B7B4-64E4FB4A2265}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="6957391" y="1352095"/>
+              <a:ext cx="238539" cy="238167"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="74" name="直線コネクタ 73">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{883FCCA8-2A64-4DEB-A44D-14AD6A7DC7C5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:endCxn id="73" idx="2"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="7195930" y="1471178"/>
+              <a:ext cx="357809" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="58" name="直線コネクタ 57">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5271DFB7-6BA9-4A87-B65A-179ACACD764B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="73" idx="1"/>
+            <a:endCxn id="73" idx="5"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="7005568" y="2152792"/>
+            <a:ext cx="168992" cy="168675"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="64" name="弦 63">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB235392-1F89-4C05-87DB-7C922CE1CC5E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="762214" flipV="1">
+            <a:off x="6998436" y="2119477"/>
+            <a:ext cx="199817" cy="168087"/>
+          </a:xfrm>
+          <a:prstGeom prst="chord">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 2700000"/>
+              <a:gd name="adj2" fmla="val 9765516"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="75" name="直線コネクタ 74">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C21EAB45-79C7-4EE9-8E0B-8763D172CA0C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="73" idx="3"/>
+            <a:endCxn id="73" idx="7"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" flipV="1">
+            <a:off x="7005568" y="2152792"/>
+            <a:ext cx="168992" cy="168675"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="76" name="直線コネクタ 75">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E157271-A069-4D20-B674-DFE1F093144D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="73" idx="0"/>
+            <a:endCxn id="73" idx="4"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7090063" y="2117858"/>
+            <a:ext cx="0" cy="238543"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>194829</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>7577</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>194829</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>44871</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="80" name="グループ化 79">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46738D50-7F74-47A8-A9ED-3D19737D1CEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2165519" y="1978267"/>
+          <a:ext cx="591207" cy="234363"/>
+          <a:chOff x="6970568" y="2117858"/>
+          <a:chExt cx="597477" cy="238543"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="81" name="グループ化 80">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A44360AD-40A7-450B-B1A3-F1BB01367D71}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="6970568" y="2117858"/>
+            <a:ext cx="597477" cy="238543"/>
+            <a:chOff x="6957391" y="1352095"/>
+            <a:chExt cx="596348" cy="238167"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="86" name="直線コネクタ 85">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE1B1229-59E2-4D1D-B464-1DB6D58CB691}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="7553739" y="1352095"/>
+              <a:ext cx="0" cy="238167"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="87" name="楕円 86">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F349569F-D9B5-4316-908E-FA77B24EA2AB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="6957391" y="1352095"/>
+              <a:ext cx="238539" cy="238167"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="88" name="直線コネクタ 87">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3037102-0B70-40C2-A0A4-F70E552F3FE7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:endCxn id="87" idx="2"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="7195930" y="1471178"/>
+              <a:ext cx="357809" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="82" name="直線コネクタ 81">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AD6FF5D-76EA-425F-8237-205BCBF91919}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="87" idx="1"/>
+            <a:endCxn id="87" idx="5"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="7005568" y="2152792"/>
+            <a:ext cx="168992" cy="168675"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="83" name="弦 82">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03E60E77-BD84-4023-817C-4D2948B1ED35}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="762214" flipV="1">
+            <a:off x="6998436" y="2119477"/>
+            <a:ext cx="199817" cy="168087"/>
+          </a:xfrm>
+          <a:prstGeom prst="chord">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 2700000"/>
+              <a:gd name="adj2" fmla="val 9765516"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>194829</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>162119</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>194830</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2343</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="89" name="グループ化 88">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C578C53-8D61-4792-89C2-6108448129B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm flipH="1">
+          <a:off x="5515691" y="753326"/>
+          <a:ext cx="591208" cy="234362"/>
+          <a:chOff x="6970568" y="2117858"/>
+          <a:chExt cx="597477" cy="238543"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="90" name="グループ化 89">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4C0A7FB-7DFB-403B-8426-9A5C12D4351F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="6970568" y="2117858"/>
+            <a:ext cx="597477" cy="238543"/>
+            <a:chOff x="6957391" y="1352095"/>
+            <a:chExt cx="596348" cy="238167"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="94" name="直線コネクタ 93">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45839B38-4CB7-4C84-A103-0C1BC26203A4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="7553739" y="1352095"/>
+              <a:ext cx="0" cy="238167"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="95" name="楕円 94">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{740CC28B-AC7E-43A6-A3DB-921082AFA25C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="6957391" y="1352095"/>
+              <a:ext cx="238539" cy="238167"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="96" name="直線コネクタ 95">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4807F397-15C4-4DA0-A0B2-F688F4FBB8CD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:endCxn id="95" idx="2"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="7195930" y="1471178"/>
+              <a:ext cx="357809" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="92" name="弦 91">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56D93D17-F538-4D9B-9117-F129C7081DC6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="762214" flipV="1">
+            <a:off x="6998436" y="2119477"/>
+            <a:ext cx="199817" cy="168087"/>
+          </a:xfrm>
+          <a:prstGeom prst="chord">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 2700000"/>
+              <a:gd name="adj2" fmla="val 9765516"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="93" name="直線コネクタ 92">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F494BE00-B1DA-4429-93FD-0CE5E036AD01}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="95" idx="3"/>
+            <a:endCxn id="95" idx="7"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" flipV="1">
+            <a:off x="7005568" y="2152792"/>
+            <a:ext cx="168992" cy="168675"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>182375</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>14076</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>181008</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>50002</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="97" name="グループ化 96">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB002BE9-9989-4F1F-B4AE-48799A427819}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="6882720" y="1984766"/>
+          <a:ext cx="589840" cy="232995"/>
+          <a:chOff x="6970568" y="2117858"/>
+          <a:chExt cx="597477" cy="238543"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="98" name="グループ化 97">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21BFEFBF-240B-4A75-865E-B01AA75F9922}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="6970568" y="2117858"/>
+            <a:ext cx="597477" cy="238543"/>
+            <a:chOff x="6957391" y="1352095"/>
+            <a:chExt cx="596348" cy="238167"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="103" name="直線コネクタ 102">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C7F8DD1-A394-4715-81D5-BB8A6962E5DB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="7553739" y="1352095"/>
+              <a:ext cx="0" cy="238167"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="104" name="楕円 103">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94438251-F342-4880-8257-1D66D5D3C8BA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="6957391" y="1352095"/>
+              <a:ext cx="238539" cy="238167"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="105" name="直線コネクタ 104">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF359C46-54A9-495F-9A16-F9E5C986FE0B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:endCxn id="104" idx="2"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="7195930" y="1471178"/>
+              <a:ext cx="357809" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="99" name="直線コネクタ 98">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A61AB92-AED3-4F79-833C-87E88F9672E0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="104" idx="1"/>
+            <a:endCxn id="104" idx="5"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="7005568" y="2152792"/>
+            <a:ext cx="168992" cy="168675"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="100" name="弦 99">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6302F1F7-AD04-43C1-B9F6-E9A98E3E1FA7}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="762214" flipV="1">
+            <a:off x="6998436" y="2119477"/>
+            <a:ext cx="199817" cy="168087"/>
+          </a:xfrm>
+          <a:prstGeom prst="chord">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 2700000"/>
+              <a:gd name="adj2" fmla="val 9765516"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="101" name="直線コネクタ 100">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E15E4B15-5A45-4777-A754-6D6F8A641B7E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="104" idx="3"/>
+            <a:endCxn id="104" idx="7"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" flipV="1">
+            <a:off x="7005568" y="2152792"/>
+            <a:ext cx="168992" cy="168675"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="102" name="直線コネクタ 101">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3AE9BC4-233A-4CED-8B0D-831080526553}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="104" idx="0"/>
+            <a:endCxn id="104" idx="4"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7090063" y="2117858"/>
+            <a:ext cx="0" cy="238543"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2244,10 +2945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:AN22"/>
+  <dimension ref="C2:AN24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="15.75"/>
@@ -2256,17 +2957,19 @@
     <col min="10" max="10" width="2.625" style="1" customWidth="1"/>
     <col min="11" max="32" width="2.625" style="1"/>
     <col min="33" max="33" width="2.625" style="1" customWidth="1"/>
-    <col min="34" max="16384" width="2.625" style="1"/>
+    <col min="34" max="38" width="2.625" style="1"/>
+    <col min="39" max="39" width="3.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="2.625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:40">
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="3:40">
       <c r="F4" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="3:40">
@@ -2274,155 +2977,196 @@
         <v>31</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="3:40">
       <c r="G7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="3:40">
       <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S10" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="W10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AF10" s="2">
         <v>21</v>
       </c>
       <c r="AI10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AN10" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="3:40">
-      <c r="AL11" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="3:40">
       <c r="M12" s="1" t="s">
-        <v>3</v>
+        <v>32</v>
+      </c>
+      <c r="AK12" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="3:40">
       <c r="C16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="AA16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI16" s="1" t="s">
-        <v>17</v>
+      <c r="AM16" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="17" spans="3:35">
+    <row r="17" spans="3:39">
       <c r="C17" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="3:39">
+      <c r="H18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="3:39">
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM19" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="3:39">
+      <c r="C20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="R17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AI17" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="3:35">
-      <c r="H18" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="3:35">
-      <c r="C19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI19" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="3:35">
-      <c r="C20" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="H20" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>0</v>
       </c>
       <c r="R20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="3:39">
+      <c r="H21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="3:39">
+      <c r="C22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AA20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI20" s="1" t="s">
-        <v>25</v>
+      <c r="R22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM22" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="21" spans="3:35">
-      <c r="H21" s="1" t="s">
-        <v>27</v>
+    <row r="23" spans="3:39">
+      <c r="C23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="22" spans="3:35">
-      <c r="C22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AI22" s="1" t="s">
-        <v>25</v>
+    <row r="24" spans="3:39">
+      <c r="C24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2437,7 +3181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F23A584-8EFB-4D7F-A3A1-CAC64E545BCA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="M43" sqref="M42:M43"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modified route control lever
</commit_message>
<xml_diff>
--- a/device/連動図表_柴山.xlsx
+++ b/device/連動図表_柴山.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED4223C-DA0D-4DD6-871D-ADB39AA6ED0F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EE7C40-3929-4616-8647-EFDF4538F996}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>3R</t>
     <phoneticPr fontId="1"/>
@@ -81,38 +81,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>幡生方～1番線</t>
-    <rPh sb="0" eb="2">
-      <t>ハタブ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>カタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>バン</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>セン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>京都方～2番線</t>
-    <rPh sb="0" eb="2">
-      <t>キョウト</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>カタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>バン</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>セン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>出発信号機</t>
     <rPh sb="0" eb="2">
       <t>シュッパツ</t>
@@ -338,18 +306,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>11L</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>11R</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>(〇31片, 〇4L片)</t>
-  </si>
-  <si>
-    <t>(〇21片, 〇3R片)</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -360,9 +317,61 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>21, 〇11L片</t>
+    <t>(〇21片, 〇2R片)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(〇31片, 〇3L片)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>21, 〇12R片</t>
     <rPh sb="8" eb="9">
       <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>12R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>21T</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>31T</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>京都方～1番線</t>
+    <rPh sb="0" eb="2">
+      <t>キョウト</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>バン</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>セン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>幡生方～2番線</t>
+    <rPh sb="0" eb="2">
+      <t>ハタブ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>バン</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>セン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -2948,7 +2957,7 @@
   <dimension ref="C2:AN24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="15.75"/>
@@ -2964,7 +2973,7 @@
   <sheetData>
     <row r="2" spans="3:40">
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="3:40">
@@ -2977,18 +2986,18 @@
         <v>31</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="3:40">
       <c r="G7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="3:40">
@@ -2999,13 +3008,13 @@
         <v>5</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AF10" s="2">
         <v>21</v>
       </c>
       <c r="AI10" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AN10" s="1" t="s">
         <v>4</v>
@@ -3013,7 +3022,7 @@
     </row>
     <row r="12" spans="3:40">
       <c r="M12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AK12" s="1" t="s">
         <v>1</v>
@@ -3021,22 +3030,22 @@
     </row>
     <row r="16" spans="3:40">
       <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="AA16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI16" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="AM16" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="3:39">
@@ -3044,50 +3053,50 @@
         <v>2</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AA17" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AI17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AM17" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="3:39">
       <c r="H18" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="3:39">
       <c r="C19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="O19" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="R19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM19" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="AA19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AI19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AM19" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="20" spans="3:39">
@@ -3095,78 +3104,84 @@
         <v>2</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>0</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="AA20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AI20" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AM20" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="3:39">
       <c r="H21" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="3:39">
       <c r="C22" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AA22" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AI22" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AM22" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="3:39">
       <c r="C23" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O23" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="R23" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="AI23" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="3:39">
       <c r="C24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>36</v>
+      <c r="O24" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="AI24" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>